<commit_message>
finished get content and download page source
</commit_message>
<xml_diff>
--- a/Netbeans/ANA-ADDIX/output/data_storage/ainow.xlsx
+++ b/Netbeans/ANA-ADDIX/output/data_storage/ainow.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RPA\ANA\ANA_2020\ANA-VIETNAM\Netbeans\ANA-ADDIX\output\data_storge\backup\Data_storage_empty\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyProjects\Sources\11. ChangeCodeANA\ANA-VIETNAM\Netbeans\ANA-ADDIX\output\data_storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2700BAB-E002-414B-A944-E9BB689ADCCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA2FA9B-1345-44C6-BD09-6CD2F839FE36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="932" firstSheet="5" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="932" firstSheet="5" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AI" sheetId="1" r:id="rId1"/>
@@ -37,18 +37,79 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="22">
   <si>
     <t>Url</t>
   </si>
   <si>
     <t>url_articles</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/05/23/170454/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/05/21/170262/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/05/20/170151/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/05/12/169561/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/05/06/169056/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/04/19/168188/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/04/14/167755/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/04/10/167574/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/03/17/165762/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/03/06/165166/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/02/26/164436/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/02/24/164207/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/02/19/163875/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/01/28/161964/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/01/16/160846/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/01/15/160768/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/01/08/160263/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2019/01/06/159978/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2018/12/27/159554/</t>
+  </si>
+  <si>
+    <t>https://ainow.ai/2018/12/26/159405/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -434,7 +495,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -463,7 +524,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -491,7 +552,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -519,7 +580,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -547,7 +608,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -575,7 +636,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -595,25 +656,125 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD93"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
+  <dimension ref="A1:A22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -631,7 +792,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -659,7 +820,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -681,11 +842,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -713,7 +874,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -741,7 +902,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -769,7 +930,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -797,7 +958,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -825,7 +986,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -853,7 +1014,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -875,11 +1036,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -907,7 +1070,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>